<commit_message>
adduser - delete - navigation testcases are executed and bug report is updated
</commit_message>
<xml_diff>
--- a/Testing/Bug Report/BugReport.xlsx
+++ b/Testing/Bug Report/BugReport.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed Mazrouaa\Documents\GitHub\learning-hub\Testing\Bug Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohammad\Documents\GitHub\learning-hub\Testing\Bug Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1E6C68-3131-41B2-AD8A-646E2608B12C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C92FB2-A091-4A7B-A05F-6230F6E5C76D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B47F1369-CBE7-4E00-A0D6-BEEA1546CCF7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{B47F1369-CBE7-4E00-A0D6-BEEA1546CCF7}"/>
   </bookViews>
   <sheets>
     <sheet name="ADD" sheetId="1" r:id="rId1"/>
+    <sheet name="AddUser" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -131,12 +132,86 @@
   <si>
     <t>Assigned</t>
   </si>
+  <si>
+    <t>BUG-AddUser-001</t>
+  </si>
+  <si>
+    <t>The admin can add users 
+with invalid email format</t>
+  </si>
+  <si>
+    <t>1-user should have a browser to navigate to signup page.
+2-User should have xampp  and it's control panel
+3- user should have the database on the phpmyadmin (reach it through xampp control panel) 
+4- open the apache server and sql server
+5-  Admin is logged in and navigated to the add user page (from navigation bar 
+select profile from the dropdown list and then 
+click add user)</t>
+  </si>
+  <si>
+    <t>admin should enter Username: "tester",
+Email: "testuser1@example",
+Password: "Abc123@",
+Confirm Password: "Abc123@"and choose
+Role: User</t>
+  </si>
+  <si>
+    <t>minor</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>M.Tarek</t>
+  </si>
+  <si>
+    <t>A validation error message should be displayed saying "Username must not contain Numbers" and the user is not added to the database.</t>
+  </si>
+  <si>
+    <t>User data is added successfully to the 
+database</t>
+  </si>
+  <si>
+    <t>22/5/2223</t>
+  </si>
+  <si>
+    <t>TC_LearningHub_adduser_005</t>
+  </si>
+  <si>
+    <t>BUG-AddUser-002</t>
+  </si>
+  <si>
+    <t>a edit profile pictrue button is 
+a exist and a circle contaning 
+text "200x200" and the admin 
+name with his role is displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-user should have a browser to navigate to signup page.
+2-User should have xampp  and it's control panel
+3- user should have the database on the phpmyadmin (reach it through xampp control panel) 
+4- open the apache server and sql server
+</t>
+  </si>
+  <si>
+    <t>1-enter admin credientials
+2- from the navigation bar elect pofile form the dropdown list then click add user</t>
+  </si>
+  <si>
+    <t>The add user page should not conatians 
+the logged admin details and the edit profile
+picture button should not be exist</t>
+  </si>
+  <si>
+    <t>The add user page conatians 
+the logged admin details and the edit profile picture button is exist</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,8 +232,49 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.5"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,8 +311,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -264,11 +386,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -291,9 +442,34 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{06F67377-BAFE-4445-B4ED-58AF6B38FCC9}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -313,15 +489,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>60960</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>365760</xdr:rowOff>
+      <xdr:rowOff>289560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1805940</xdr:colOff>
+      <xdr:colOff>1866900</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1531620</xdr:rowOff>
+      <xdr:rowOff>1455420</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -344,8 +520,63 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17838420" y="769620"/>
+          <a:off x="17899380" y="693420"/>
           <a:ext cx="1805940" cy="1165860"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>365761</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>206432</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>3368040</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>3357617</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C68D5D01-5CCF-8097-9331-7CEDC3495E1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19179541" y="2926772"/>
+          <a:ext cx="3002279" cy="3151185"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -656,11 +887,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{498577AC-8506-48C6-8803-AB5E96FC3B0E}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20.109375" customWidth="1"/>
     <col min="2" max="2" width="37.5546875" customWidth="1"/>
@@ -679,7 +910,7 @@
     <col min="15" max="15" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="16.2" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -726,7 +957,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="155.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="155.4" customHeight="1" thickBot="1">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -780,4 +1011,177 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50A8F9C3-99D9-4F67-B67B-D861EE406BC3}">
+  <dimension ref="A1:O3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="4" width="43.77734375" customWidth="1"/>
+    <col min="5" max="5" width="35.77734375" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" customWidth="1"/>
+    <col min="9" max="9" width="21.109375" customWidth="1"/>
+    <col min="10" max="10" width="39.6640625" customWidth="1"/>
+    <col min="11" max="11" width="36" customWidth="1"/>
+    <col min="12" max="12" width="55.5546875" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" customWidth="1"/>
+    <col min="14" max="14" width="26" customWidth="1"/>
+    <col min="15" max="15" width="20.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="15.6">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="198.6" customHeight="1">
+      <c r="A2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="10"/>
+      <c r="M2" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="285.60000000000002" customHeight="1">
+      <c r="A3" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3" s="10"/>
+      <c r="M3" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="11"/>
+      <c r="O3" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O3" xr:uid="{7CFEF66A-BE28-4677-B841-C333651717DD}">
+      <formula1>"New,Assigned,Fixed,Re-test,Re-open,close"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>